<commit_message>
Troca de sitema operacional no meu computador
</commit_message>
<xml_diff>
--- a/Examples/teste_example_2/data_exa.xlsx
+++ b/Examples/teste_example_2/data_exa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\PycharmProjects\MT_PEU\Examples\teste_example_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\PycharmProjects\MT_PEU\Examples\teste_example_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1D9F84-D1CE-4477-9860-8D851ADC143F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C24DA6-F6EE-474A-98B6-85DE5A535428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Y</t>
   </si>
@@ -39,6 +39,129 @@
   </si>
   <si>
     <t>Uxtemperature</t>
+  </si>
+  <si>
+    <t>60.1</t>
+  </si>
+  <si>
+    <t>45.1</t>
+  </si>
+  <si>
+    <t>90.4</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.949</t>
+  </si>
+  <si>
+    <t>0.886</t>
+  </si>
+  <si>
+    <t>0.785</t>
+  </si>
+  <si>
+    <t>0.791</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>0.787</t>
+  </si>
+  <si>
+    <t>0.877</t>
+  </si>
+  <si>
+    <t>0.938</t>
+  </si>
+  <si>
+    <t>0.782</t>
+  </si>
+  <si>
+    <t>0.827</t>
+  </si>
+  <si>
+    <t>0.696</t>
+  </si>
+  <si>
+    <t>0.582</t>
+  </si>
+  <si>
+    <t>0.795</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.79</t>
+  </si>
+  <si>
+    <t>0.883</t>
+  </si>
+  <si>
+    <t>0.712</t>
+  </si>
+  <si>
+    <t>0.576</t>
+  </si>
+  <si>
+    <t>0.715</t>
+  </si>
+  <si>
+    <t>0.673</t>
+  </si>
+  <si>
+    <t>0.802</t>
+  </si>
+  <si>
+    <t>0.804</t>
+  </si>
+  <si>
+    <t>0.794</t>
+  </si>
+  <si>
+    <t>0.799</t>
+  </si>
+  <si>
+    <t>0.764</t>
+  </si>
+  <si>
+    <t>0.688</t>
+  </si>
+  <si>
+    <t>0.717</t>
+  </si>
+  <si>
+    <t>0.695</t>
+  </si>
+  <si>
+    <t>0.808</t>
+  </si>
+  <si>
+    <t>0.655</t>
+  </si>
+  <si>
+    <t>0.309</t>
+  </si>
+  <si>
+    <t>0.689</t>
+  </si>
+  <si>
+    <t>0.437</t>
+  </si>
+  <si>
+    <t>0.425</t>
+  </si>
+  <si>
+    <t>0.638</t>
+  </si>
+  <si>
+    <t>0.659</t>
+  </si>
+  <si>
+    <t>0.449</t>
   </si>
 </sst>
 </file>
@@ -310,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78D95B7-B7C2-4B1D-A0AA-907023D16FAD}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -471,8 +594,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>45.1</v>
+      <c r="A12" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -597,8 +720,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>90.4</v>
+      <c r="A21" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -723,8 +846,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>45.1</v>
+      <c r="A30" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
@@ -835,8 +958,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>60.1</v>
+      <c r="A38" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -917,8 +1040,8 @@
   </sheetPr>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -932,120 +1055,120 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0.9</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>0.94899999999999995</v>
+      <c r="A3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>0.88600000000000001</v>
+      <c r="A4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>0.78500000000000003</v>
+      <c r="A5" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>0.79100000000000004</v>
+      <c r="A6" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>0.89</v>
+      <c r="A7" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>0.78700000000000003</v>
+      <c r="A8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>0.877</v>
+      <c r="A9" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>0.93799999999999994</v>
+      <c r="A10" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>0.78200000000000003</v>
+      <c r="A11" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>0.82699999999999996</v>
+      <c r="A12" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>0.69599999999999995</v>
+      <c r="A13" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>0.58199999999999996</v>
+      <c r="A14" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>0.79500000000000004</v>
+      <c r="A15" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>0.8</v>
+      <c r="A16" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -1053,208 +1176,208 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>0.79</v>
+      <c r="A17" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>0.88300000000000001</v>
+      <c r="A18" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>0.71199999999999997</v>
+      <c r="A19" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>0.57599999999999996</v>
+      <c r="A20" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>0.71499999999999997</v>
+      <c r="A21" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>0.67300000000000004</v>
+      <c r="A22" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>0.80200000000000005</v>
+      <c r="A23" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>0.80200000000000005</v>
+      <c r="A24" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>0.80400000000000005</v>
+      <c r="A25" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>0.79400000000000004</v>
+      <c r="A26" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>0.80400000000000005</v>
+      <c r="A27" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>0.79900000000000004</v>
+      <c r="A28" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>0.76400000000000001</v>
+      <c r="A29" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>0.68799999999999994</v>
+      <c r="A30" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>0.71699999999999997</v>
+      <c r="A31" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>0.80200000000000005</v>
+      <c r="A32" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>0.69499999999999995</v>
+      <c r="A33" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>0.80800000000000005</v>
+      <c r="A34" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>0.65500000000000003</v>
+      <c r="A35" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>0.309</v>
+      <c r="A36" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>0.68899999999999995</v>
+      <c r="A37" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>0.437</v>
+      <c r="A38" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>0.42499999999999999</v>
+      <c r="A39" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>0.63800000000000001</v>
+      <c r="A40" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>0.65900000000000003</v>
+      <c r="A41" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>0.44900000000000001</v>
+      <c r="A42" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Revert "Troca de sitema operacional no meu computador"
This reverts commit 8abe3fcb9522c906a2be6f48f974b3a87f40a922.
</commit_message>
<xml_diff>
--- a/Examples/teste_example_2/data_exa.xlsx
+++ b/Examples/teste_example_2/data_exa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\PycharmProjects\MT_PEU\Examples\teste_example_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\PycharmProjects\MT_PEU\Examples\teste_example_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C24DA6-F6EE-474A-98B6-85DE5A535428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1D9F84-D1CE-4477-9860-8D851ADC143F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Y</t>
   </si>
@@ -39,129 +39,6 @@
   </si>
   <si>
     <t>Uxtemperature</t>
-  </si>
-  <si>
-    <t>60.1</t>
-  </si>
-  <si>
-    <t>45.1</t>
-  </si>
-  <si>
-    <t>90.4</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>0.949</t>
-  </si>
-  <si>
-    <t>0.886</t>
-  </si>
-  <si>
-    <t>0.785</t>
-  </si>
-  <si>
-    <t>0.791</t>
-  </si>
-  <si>
-    <t>0.89</t>
-  </si>
-  <si>
-    <t>0.787</t>
-  </si>
-  <si>
-    <t>0.877</t>
-  </si>
-  <si>
-    <t>0.938</t>
-  </si>
-  <si>
-    <t>0.782</t>
-  </si>
-  <si>
-    <t>0.827</t>
-  </si>
-  <si>
-    <t>0.696</t>
-  </si>
-  <si>
-    <t>0.582</t>
-  </si>
-  <si>
-    <t>0.795</t>
-  </si>
-  <si>
-    <t>0.8</t>
-  </si>
-  <si>
-    <t>0.79</t>
-  </si>
-  <si>
-    <t>0.883</t>
-  </si>
-  <si>
-    <t>0.712</t>
-  </si>
-  <si>
-    <t>0.576</t>
-  </si>
-  <si>
-    <t>0.715</t>
-  </si>
-  <si>
-    <t>0.673</t>
-  </si>
-  <si>
-    <t>0.802</t>
-  </si>
-  <si>
-    <t>0.804</t>
-  </si>
-  <si>
-    <t>0.794</t>
-  </si>
-  <si>
-    <t>0.799</t>
-  </si>
-  <si>
-    <t>0.764</t>
-  </si>
-  <si>
-    <t>0.688</t>
-  </si>
-  <si>
-    <t>0.717</t>
-  </si>
-  <si>
-    <t>0.695</t>
-  </si>
-  <si>
-    <t>0.808</t>
-  </si>
-  <si>
-    <t>0.655</t>
-  </si>
-  <si>
-    <t>0.309</t>
-  </si>
-  <si>
-    <t>0.689</t>
-  </si>
-  <si>
-    <t>0.437</t>
-  </si>
-  <si>
-    <t>0.425</t>
-  </si>
-  <si>
-    <t>0.638</t>
-  </si>
-  <si>
-    <t>0.659</t>
-  </si>
-  <si>
-    <t>0.449</t>
   </si>
 </sst>
 </file>
@@ -433,8 +310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78D95B7-B7C2-4B1D-A0AA-907023D16FAD}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -594,8 +471,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
+      <c r="A12" s="2">
+        <v>45.1</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -720,8 +597,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>8</v>
+      <c r="A21" s="2">
+        <v>90.4</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -846,8 +723,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>7</v>
+      <c r="A30" s="2">
+        <v>45.1</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
@@ -958,8 +835,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>6</v>
+      <c r="A38" s="2">
+        <v>60.1</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -1040,8 +917,8 @@
   </sheetPr>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1055,120 +932,120 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
+      <c r="A2" s="1">
+        <v>0.9</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
+      <c r="A3" s="1">
+        <v>0.94899999999999995</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
+      <c r="A4" s="1">
+        <v>0.88600000000000001</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
+      <c r="A5" s="1">
+        <v>0.78500000000000003</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
+      <c r="A6" s="1">
+        <v>0.79100000000000004</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
+      <c r="A7" s="1">
+        <v>0.89</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
+      <c r="A8" s="1">
+        <v>0.78700000000000003</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
+      <c r="A9" s="1">
+        <v>0.877</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
+      <c r="A10" s="1">
+        <v>0.93799999999999994</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
+      <c r="A11" s="1">
+        <v>0.78200000000000003</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
+      <c r="A12" s="1">
+        <v>0.82699999999999996</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
+      <c r="A13" s="1">
+        <v>0.69599999999999995</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
+      <c r="A14" s="1">
+        <v>0.58199999999999996</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
+      <c r="A15" s="1">
+        <v>0.79500000000000004</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
+      <c r="A16" s="1">
+        <v>0.8</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -1176,208 +1053,208 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
+      <c r="A17" s="1">
+        <v>0.79</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
+      <c r="A18" s="1">
+        <v>0.88300000000000001</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
+      <c r="A19" s="1">
+        <v>0.71199999999999997</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>27</v>
+      <c r="A20" s="1">
+        <v>0.57599999999999996</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>28</v>
+      <c r="A21" s="1">
+        <v>0.71499999999999997</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>29</v>
+      <c r="A22" s="1">
+        <v>0.67300000000000004</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>30</v>
+      <c r="A23" s="1">
+        <v>0.80200000000000005</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>30</v>
+      <c r="A24" s="1">
+        <v>0.80200000000000005</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
+      <c r="A25" s="1">
+        <v>0.80400000000000005</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
+      <c r="A26" s="1">
+        <v>0.79400000000000004</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>31</v>
+      <c r="A27" s="1">
+        <v>0.80400000000000005</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>33</v>
+      <c r="A28" s="1">
+        <v>0.79900000000000004</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>34</v>
+      <c r="A29" s="1">
+        <v>0.76400000000000001</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>35</v>
+      <c r="A30" s="1">
+        <v>0.68799999999999994</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>36</v>
+      <c r="A31" s="1">
+        <v>0.71699999999999997</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>30</v>
+      <c r="A32" s="1">
+        <v>0.80200000000000005</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>37</v>
+      <c r="A33" s="1">
+        <v>0.69499999999999995</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>38</v>
+      <c r="A34" s="1">
+        <v>0.80800000000000005</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>39</v>
+      <c r="A35" s="1">
+        <v>0.65500000000000003</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>40</v>
+      <c r="A36" s="1">
+        <v>0.309</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>41</v>
+      <c r="A37" s="1">
+        <v>0.68899999999999995</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>42</v>
+      <c r="A38" s="1">
+        <v>0.437</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>43</v>
+      <c r="A39" s="1">
+        <v>0.42499999999999999</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>44</v>
+      <c r="A40" s="1">
+        <v>0.63800000000000001</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>45</v>
+      <c r="A41" s="1">
+        <v>0.65900000000000003</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>46</v>
+      <c r="A42" s="1">
+        <v>0.44900000000000001</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Atualização dos exemplos *Exemplos atualizados para obedecer as alterações na entrada de dados
</commit_message>
<xml_diff>
--- a/Examples/teste_example_2/data_exa.xlsx
+++ b/Examples/teste_example_2/data_exa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\PycharmProjects\MT_PEU\Examples\teste_example_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\PycharmProjects\MT_PEU\Examples\teste_example_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1D9F84-D1CE-4477-9860-8D851ADC143F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C24DA6-F6EE-474A-98B6-85DE5A535428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Y</t>
   </si>
@@ -39,6 +39,129 @@
   </si>
   <si>
     <t>Uxtemperature</t>
+  </si>
+  <si>
+    <t>60.1</t>
+  </si>
+  <si>
+    <t>45.1</t>
+  </si>
+  <si>
+    <t>90.4</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.949</t>
+  </si>
+  <si>
+    <t>0.886</t>
+  </si>
+  <si>
+    <t>0.785</t>
+  </si>
+  <si>
+    <t>0.791</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>0.787</t>
+  </si>
+  <si>
+    <t>0.877</t>
+  </si>
+  <si>
+    <t>0.938</t>
+  </si>
+  <si>
+    <t>0.782</t>
+  </si>
+  <si>
+    <t>0.827</t>
+  </si>
+  <si>
+    <t>0.696</t>
+  </si>
+  <si>
+    <t>0.582</t>
+  </si>
+  <si>
+    <t>0.795</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.79</t>
+  </si>
+  <si>
+    <t>0.883</t>
+  </si>
+  <si>
+    <t>0.712</t>
+  </si>
+  <si>
+    <t>0.576</t>
+  </si>
+  <si>
+    <t>0.715</t>
+  </si>
+  <si>
+    <t>0.673</t>
+  </si>
+  <si>
+    <t>0.802</t>
+  </si>
+  <si>
+    <t>0.804</t>
+  </si>
+  <si>
+    <t>0.794</t>
+  </si>
+  <si>
+    <t>0.799</t>
+  </si>
+  <si>
+    <t>0.764</t>
+  </si>
+  <si>
+    <t>0.688</t>
+  </si>
+  <si>
+    <t>0.717</t>
+  </si>
+  <si>
+    <t>0.695</t>
+  </si>
+  <si>
+    <t>0.808</t>
+  </si>
+  <si>
+    <t>0.655</t>
+  </si>
+  <si>
+    <t>0.309</t>
+  </si>
+  <si>
+    <t>0.689</t>
+  </si>
+  <si>
+    <t>0.437</t>
+  </si>
+  <si>
+    <t>0.425</t>
+  </si>
+  <si>
+    <t>0.638</t>
+  </si>
+  <si>
+    <t>0.659</t>
+  </si>
+  <si>
+    <t>0.449</t>
   </si>
 </sst>
 </file>
@@ -310,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78D95B7-B7C2-4B1D-A0AA-907023D16FAD}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -471,8 +594,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>45.1</v>
+      <c r="A12" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -597,8 +720,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>90.4</v>
+      <c r="A21" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -723,8 +846,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>45.1</v>
+      <c r="A30" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
@@ -835,8 +958,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>60.1</v>
+      <c r="A38" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -917,8 +1040,8 @@
   </sheetPr>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -932,120 +1055,120 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0.9</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>0.94899999999999995</v>
+      <c r="A3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>0.88600000000000001</v>
+      <c r="A4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>0.78500000000000003</v>
+      <c r="A5" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>0.79100000000000004</v>
+      <c r="A6" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>0.89</v>
+      <c r="A7" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>0.78700000000000003</v>
+      <c r="A8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>0.877</v>
+      <c r="A9" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>0.93799999999999994</v>
+      <c r="A10" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>0.78200000000000003</v>
+      <c r="A11" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>0.82699999999999996</v>
+      <c r="A12" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>0.69599999999999995</v>
+      <c r="A13" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>0.58199999999999996</v>
+      <c r="A14" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>0.79500000000000004</v>
+      <c r="A15" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>0.8</v>
+      <c r="A16" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -1053,208 +1176,208 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>0.79</v>
+      <c r="A17" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>0.88300000000000001</v>
+      <c r="A18" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>0.71199999999999997</v>
+      <c r="A19" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>0.57599999999999996</v>
+      <c r="A20" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>0.71499999999999997</v>
+      <c r="A21" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>0.67300000000000004</v>
+      <c r="A22" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>0.80200000000000005</v>
+      <c r="A23" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>0.80200000000000005</v>
+      <c r="A24" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>0.80400000000000005</v>
+      <c r="A25" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>0.79400000000000004</v>
+      <c r="A26" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>0.80400000000000005</v>
+      <c r="A27" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>0.79900000000000004</v>
+      <c r="A28" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>0.76400000000000001</v>
+      <c r="A29" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>0.68799999999999994</v>
+      <c r="A30" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>0.71699999999999997</v>
+      <c r="A31" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>0.80200000000000005</v>
+      <c r="A32" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>0.69499999999999995</v>
+      <c r="A33" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>0.80800000000000005</v>
+      <c r="A34" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>0.65500000000000003</v>
+      <c r="A35" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>0.309</v>
+      <c r="A36" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>0.68899999999999995</v>
+      <c r="A37" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>0.437</v>
+      <c r="A38" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>0.42499999999999999</v>
+      <c r="A39" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>0.63800000000000001</v>
+      <c r="A40" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>0.65900000000000003</v>
+      <c r="A41" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>0.44900000000000001</v>
+      <c r="A42" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>

</xml_diff>